<commit_message>
support to add the hide cell jishi pay
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="工资明细" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,13 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">工资明细!$A$1:$P$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -45,7 +52,7 @@
     <t xml:space="preserve">绩效奖金</t>
   </si>
   <si>
-    <t xml:space="preserve">及时奖励</t>
+    <t xml:space="preserve">及时激励</t>
   </si>
   <si>
     <t xml:space="preserve">就餐补贴</t>
@@ -85,10 +92,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
     <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -185,7 +193,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,6 +227,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,28 +313,26 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q183" activeCellId="0" sqref="Q183"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.75348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2139534883721"/>
-    <col collapsed="false" hidden="true" max="6" min="6" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="1" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.4"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="1021" min="19" style="1" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="1" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="103.125581395349"/>
+    <col collapsed="false" hidden="false" max="1021" min="19" style="1" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -381,7 +391,11 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="51.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="51.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N2" s="9" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.251388888888889" right="0.251388888888889" top="0.357638888888889" bottom="0.160416666666667" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>